<commit_message>
🩹 template format update, minor
</commit_message>
<xml_diff>
--- a/template/NSE Option Chain.xlsx
+++ b/template/NSE Option Chain.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AlgoTrading\notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AlgoTrading\Python Modules (iTraders - GitHub)\nseoptions\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7940927-D798-4563-AEBE-611856D803FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8C388A-DA06-4483-8995-59653C9430BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1130,6 +1130,39 @@
     <xf numFmtId="165" fontId="4" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1137,6 +1170,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1173,48 +1215,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1873,8 +1873,8 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12" style="14" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="4" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="14.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.77734375" style="4" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="14.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.21875" style="3" bestFit="1" customWidth="1"/>
@@ -1895,9 +1895,8 @@
     <col min="24" max="24" width="11.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14.6640625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="12.77734375" style="4" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="12" style="14" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12" style="14" customWidth="1"/>
+    <col min="27" max="27" width="12.77734375" style="4" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="29" width="12" style="14" customWidth="1"/>
     <col min="30" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -2088,161 +2087,161 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="111" customFormat="1" ht="12" x14ac:dyDescent="0.3">
-      <c r="A5" s="106" t="s">
+    <row r="5" spans="1:29" s="95" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="A5" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="106" t="s">
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="107"/>
-      <c r="M5" s="107"/>
-      <c r="N5" s="108"/>
-      <c r="O5" s="109"/>
-      <c r="P5" s="110"/>
-      <c r="Q5" s="107"/>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="107"/>
-      <c r="Y5" s="107"/>
-      <c r="Z5" s="106" t="s">
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="93"/>
+      <c r="O5" s="105"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="92"/>
+      <c r="S5" s="92"/>
+      <c r="T5" s="92"/>
+      <c r="U5" s="92"/>
+      <c r="V5" s="92"/>
+      <c r="W5" s="92"/>
+      <c r="X5" s="92"/>
+      <c r="Y5" s="92"/>
+      <c r="Z5" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="AA5" s="107"/>
-      <c r="AB5" s="107"/>
-      <c r="AC5" s="106" t="s">
+      <c r="AA5" s="92"/>
+      <c r="AB5" s="92"/>
+      <c r="AC5" s="91" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="111" customFormat="1" ht="12" x14ac:dyDescent="0.3">
-      <c r="A6" s="112" t="e">
+    <row r="6" spans="1:29" s="95" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="A6" s="96" t="e">
         <f>'OC Profile'!$A$4-'OC Profile'!$A$5</f>
         <v>#NUM!</v>
       </c>
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
-      <c r="D6" s="112" t="e">
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="96" t="e">
         <f>'OC Profile'!$E$4-'OC Profile'!$E$5</f>
         <v>#NUM!</v>
       </c>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="107"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="107"/>
-      <c r="L6" s="107"/>
-      <c r="M6" s="107"/>
-      <c r="N6" s="108"/>
-      <c r="O6" s="113"/>
-      <c r="P6" s="110"/>
-      <c r="Q6" s="107"/>
-      <c r="R6" s="107"/>
-      <c r="S6" s="107"/>
-      <c r="T6" s="107"/>
-      <c r="U6" s="107"/>
-      <c r="V6" s="107"/>
-      <c r="W6" s="107"/>
-      <c r="X6" s="107"/>
-      <c r="Y6" s="107"/>
-      <c r="Z6" s="112" t="e">
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="106"/>
+      <c r="P6" s="94"/>
+      <c r="Q6" s="92"/>
+      <c r="R6" s="92"/>
+      <c r="S6" s="92"/>
+      <c r="T6" s="92"/>
+      <c r="U6" s="92"/>
+      <c r="V6" s="92"/>
+      <c r="W6" s="92"/>
+      <c r="X6" s="92"/>
+      <c r="Y6" s="92"/>
+      <c r="Z6" s="96" t="e">
         <f>'OC Profile'!$K$4-'OC Profile'!$K$5</f>
         <v>#NUM!</v>
       </c>
-      <c r="AA6" s="107"/>
-      <c r="AB6" s="107"/>
-      <c r="AC6" s="112" t="e">
+      <c r="AA6" s="92"/>
+      <c r="AB6" s="92"/>
+      <c r="AC6" s="96" t="e">
         <f>'OC Profile'!$G$4-'OC Profile'!$G$5</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="111" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="114" t="e">
+    <row r="7" spans="1:29" s="95" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="97" t="e">
         <f>'OC Profile'!$A$5-'OC Profile'!$A$6</f>
         <v>#NUM!</v>
       </c>
-      <c r="B7" s="115"/>
-      <c r="C7" s="115"/>
-      <c r="D7" s="114" t="e">
+      <c r="B7" s="98"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="97" t="e">
         <f>'OC Profile'!$E$5-'OC Profile'!$E$6</f>
         <v>#NUM!</v>
       </c>
-      <c r="E7" s="115"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="115"/>
-      <c r="M7" s="115"/>
-      <c r="N7" s="116"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="118"/>
-      <c r="Q7" s="115"/>
-      <c r="R7" s="115"/>
-      <c r="S7" s="115"/>
-      <c r="T7" s="115"/>
-      <c r="U7" s="115"/>
-      <c r="V7" s="115"/>
-      <c r="W7" s="115"/>
-      <c r="X7" s="115"/>
-      <c r="Y7" s="115"/>
-      <c r="Z7" s="114" t="e">
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="99"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="100"/>
+      <c r="Q7" s="98"/>
+      <c r="R7" s="98"/>
+      <c r="S7" s="98"/>
+      <c r="T7" s="98"/>
+      <c r="U7" s="98"/>
+      <c r="V7" s="98"/>
+      <c r="W7" s="98"/>
+      <c r="X7" s="98"/>
+      <c r="Y7" s="98"/>
+      <c r="Z7" s="97" t="e">
         <f>'OC Profile'!$K$5-'OC Profile'!$K$6</f>
         <v>#NUM!</v>
       </c>
-      <c r="AA7" s="115"/>
-      <c r="AB7" s="115"/>
-      <c r="AC7" s="114" t="e">
+      <c r="AA7" s="98"/>
+      <c r="AB7" s="98"/>
+      <c r="AC7" s="97" t="e">
         <f>'OC Profile'!$G$5-'OC Profile'!$G$6</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="111" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="112"/>
-      <c r="B8" s="107"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
-      <c r="K8" s="107"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="107"/>
-      <c r="N8" s="108"/>
-      <c r="O8" s="119"/>
-      <c r="P8" s="110"/>
-      <c r="Q8" s="107"/>
-      <c r="R8" s="107"/>
-      <c r="S8" s="107"/>
-      <c r="T8" s="107"/>
-      <c r="U8" s="107"/>
-      <c r="V8" s="107"/>
-      <c r="W8" s="107"/>
-      <c r="X8" s="107"/>
-      <c r="Y8" s="107"/>
-      <c r="Z8" s="112"/>
-      <c r="AA8" s="107"/>
-      <c r="AB8" s="107"/>
-      <c r="AC8" s="112"/>
+    <row r="8" spans="1:29" s="95" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="96"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="92"/>
+      <c r="N8" s="93"/>
+      <c r="O8" s="101"/>
+      <c r="P8" s="94"/>
+      <c r="Q8" s="92"/>
+      <c r="R8" s="92"/>
+      <c r="S8" s="92"/>
+      <c r="T8" s="92"/>
+      <c r="U8" s="92"/>
+      <c r="V8" s="92"/>
+      <c r="W8" s="92"/>
+      <c r="X8" s="92"/>
+      <c r="Y8" s="92"/>
+      <c r="Z8" s="96"/>
+      <c r="AA8" s="92"/>
+      <c r="AB8" s="92"/>
+      <c r="AC8" s="96"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="24"/>
@@ -2276,41 +2275,41 @@
       <c r="AC9" s="24"/>
     </row>
     <row r="10" spans="1:29" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="91" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="91"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="91"/>
-      <c r="L10" s="91"/>
-      <c r="M10" s="91"/>
-      <c r="N10" s="91"/>
-      <c r="O10" s="92" t="s">
+      <c r="A10" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="102"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="P10" s="91" t="s">
+      <c r="P10" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="Q10" s="91"/>
-      <c r="R10" s="91"/>
-      <c r="S10" s="91"/>
-      <c r="T10" s="91"/>
-      <c r="U10" s="91"/>
-      <c r="V10" s="91"/>
-      <c r="W10" s="91"/>
-      <c r="X10" s="91"/>
-      <c r="Y10" s="91"/>
-      <c r="Z10" s="91"/>
-      <c r="AA10" s="91"/>
-      <c r="AB10" s="91"/>
-      <c r="AC10" s="91"/>
+      <c r="Q10" s="102"/>
+      <c r="R10" s="102"/>
+      <c r="S10" s="102"/>
+      <c r="T10" s="102"/>
+      <c r="U10" s="102"/>
+      <c r="V10" s="102"/>
+      <c r="W10" s="102"/>
+      <c r="X10" s="102"/>
+      <c r="Y10" s="102"/>
+      <c r="Z10" s="102"/>
+      <c r="AA10" s="102"/>
+      <c r="AB10" s="102"/>
+      <c r="AC10" s="102"/>
     </row>
     <row r="11" spans="1:29" s="18" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
@@ -2355,7 +2354,7 @@
       <c r="N11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="93"/>
+      <c r="O11" s="104"/>
       <c r="P11" s="22" t="s">
         <v>11</v>
       </c>
@@ -3679,72 +3678,96 @@
     <mergeCell ref="O5:O7"/>
   </mergeCells>
   <conditionalFormatting sqref="A33:A52">
-    <cfRule type="top10" dxfId="31" priority="32" rank="1"/>
-    <cfRule type="top10" dxfId="30" priority="33" rank="2"/>
-    <cfRule type="top10" dxfId="29" priority="34" rank="3"/>
+    <cfRule type="top10" dxfId="31" priority="34" rank="1"/>
+    <cfRule type="top10" dxfId="30" priority="35" rank="2"/>
+    <cfRule type="top10" dxfId="29" priority="36" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B4 D3:D4 Z3:Z4 AB3:AC4">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="greaterThan">
       <formula>0.93</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
       <formula>0.83</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="greaterThan">
       <formula>0.75</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="lessThan">
       <formula>0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:B52">
-    <cfRule type="top10" dxfId="24" priority="20" rank="1"/>
-    <cfRule type="top10" dxfId="23" priority="21" rank="2"/>
-    <cfRule type="top10" dxfId="22" priority="22" rank="3"/>
+    <cfRule type="top10" dxfId="24" priority="22" rank="1"/>
+    <cfRule type="top10" dxfId="23" priority="23" rank="2"/>
+    <cfRule type="top10" dxfId="22" priority="24" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:D52">
-    <cfRule type="top10" dxfId="21" priority="26" rank="1"/>
-    <cfRule type="top10" dxfId="20" priority="27" rank="2"/>
-    <cfRule type="top10" dxfId="19" priority="28" rank="3"/>
+    <cfRule type="top10" dxfId="21" priority="28" rank="1"/>
+    <cfRule type="top10" dxfId="20" priority="29" rank="2"/>
+    <cfRule type="top10" dxfId="19" priority="30" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E52 Y12:Y52">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O4">
-    <cfRule type="cellIs" dxfId="17" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="between">
       <formula>0.9</formula>
       <formula>1.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThan">
       <formula>0.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
       <formula>1.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z12:Z32">
-    <cfRule type="top10" dxfId="8" priority="23" rank="1"/>
-    <cfRule type="top10" dxfId="7" priority="24" rank="2"/>
-    <cfRule type="top10" dxfId="6" priority="25" rank="3"/>
+    <cfRule type="top10" dxfId="8" priority="25" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="26" rank="2"/>
+    <cfRule type="top10" dxfId="6" priority="27" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB12:AB32">
-    <cfRule type="top10" dxfId="5" priority="17" rank="1"/>
-    <cfRule type="top10" dxfId="4" priority="18" rank="2"/>
-    <cfRule type="top10" dxfId="3" priority="19" rank="3"/>
+    <cfRule type="top10" dxfId="5" priority="19" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="20" rank="2"/>
+    <cfRule type="top10" dxfId="3" priority="21" rank="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC12:AC32">
-    <cfRule type="top10" dxfId="2" priority="29" rank="1"/>
-    <cfRule type="top10" dxfId="1" priority="30" rank="2"/>
-    <cfRule type="top10" dxfId="0" priority="31" rank="3"/>
+    <cfRule type="top10" dxfId="2" priority="31" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="32" rank="2"/>
+    <cfRule type="top10" dxfId="0" priority="33" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C42">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="-2.5"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="2.5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA22:AA42">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="-2.5"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="2.5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{1249B104-FCA3-4408-86EB-A3EDEEFA8C1C}">
+          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{1249B104-FCA3-4408-86EB-A3EDEEFA8C1C}">
             <xm:f>'OC Profile'!$O$6</xm:f>
             <x14:dxf>
               <font>
@@ -3757,7 +3780,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{8D344422-8EFF-455E-BD20-26D7E7FA6C2C}">
+          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{8D344422-8EFF-455E-BD20-26D7E7FA6C2C}">
             <xm:f>'OC Profile'!$O$5</xm:f>
             <x14:dxf>
               <font>
@@ -3770,7 +3793,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{619B2F65-148B-4911-AA3C-796F860FEADA}">
+          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{619B2F65-148B-4911-AA3C-796F860FEADA}">
             <xm:f>'OC Profile'!$O$4</xm:f>
             <x14:dxf>
               <font>
@@ -3786,7 +3809,7 @@
           <xm:sqref>O12:O32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{95419161-3E50-4B21-A92F-5C54FFA3A5B2}">
+          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{95419161-3E50-4B21-A92F-5C54FFA3A5B2}">
             <xm:f>'OC Profile'!$N$6</xm:f>
             <x14:dxf>
               <font>
@@ -3799,7 +3822,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{3028D5F8-4D87-4BCD-A65B-E299A7F3998C}">
+          <x14:cfRule type="cellIs" priority="14" operator="equal" id="{3028D5F8-4D87-4BCD-A65B-E299A7F3998C}">
             <xm:f>'OC Profile'!$N$5</xm:f>
             <x14:dxf>
               <font>
@@ -3812,7 +3835,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{1C3E22D3-0E43-47A6-B6F3-81A2587E73D9}">
+          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{1C3E22D3-0E43-47A6-B6F3-81A2587E73D9}">
             <xm:f>'OC Profile'!$N$4</xm:f>
             <x14:dxf>
               <font>
@@ -3895,50 +3918,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="Q1" s="96" t="s">
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="109"/>
+      <c r="Q1" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="97"/>
+      <c r="R1" s="111"/>
     </row>
     <row r="2" spans="1:18" s="29" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="94" t="s">
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="99"/>
+      <c r="Q2" s="112"/>
+      <c r="R2" s="113"/>
     </row>
     <row r="3" spans="1:18" s="29" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
@@ -3983,7 +4006,7 @@
       <c r="N3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="94"/>
+      <c r="O3" s="108"/>
       <c r="Q3" s="73"/>
       <c r="R3" s="73" t="s">
         <v>26</v>
@@ -5346,44 +5369,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="28" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="102"/>
-      <c r="N1" s="96" t="s">
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="116"/>
+      <c r="N1" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="97"/>
+      <c r="O1" s="111"/>
     </row>
     <row r="2" spans="1:15" s="18" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="103" t="s">
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="105"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="99"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="119"/>
+      <c r="N2" s="112"/>
+      <c r="O2" s="113"/>
     </row>
     <row r="3" spans="1:15" s="18" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="35" t="s">

</xml_diff>

<commit_message>
🩹 ignore all contents of output, update template with iv sparklines
</commit_message>
<xml_diff>
--- a/template/NSE Option Chain.xlsx
+++ b/template/NSE Option Chain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AlgoTrading\Python Modules (iTraders - GitHub)\nseoptions\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8C388A-DA06-4483-8995-59653C9430BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5460BF7-26E9-498A-9B14-445296B6B5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>CALL</t>
   </si>
@@ -153,18 +153,25 @@
       <t>(min. of the three metric)</t>
     </r>
   </si>
+  <si>
+    <t>ITM</t>
+  </si>
+  <si>
+    <t>OTM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +275,15 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,8 +374,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="37">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -863,6 +883,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -870,7 +941,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1067,9 +1138,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1100,9 +1168,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1118,9 +1183,6 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="3" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1163,6 +1225,27 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1179,6 +1262,114 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1215,6 +1406,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1265,17 +1462,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1288,6 +1474,17 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1537,17 +1734,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1560,6 +1746,17 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1884,7 +2081,7 @@
     <col min="11" max="12" width="9.6640625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="13" max="13" width="9.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="11.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.6640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="19.77734375" style="5" customWidth="1"/>
     <col min="16" max="16" width="11.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.6640625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -1902,36 +2099,36 @@
   <sheetData>
     <row r="1" spans="1:29" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="67"/>
-      <c r="B1" s="90">
+      <c r="B1" s="87">
         <f>SUM(B$23:B$42)</f>
         <v>0</v>
       </c>
       <c r="C1" s="69"/>
       <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="69"/>
       <c r="I1" s="68"/>
       <c r="J1" s="68"/>
       <c r="K1" s="68"/>
       <c r="L1" s="68"/>
       <c r="M1" s="68"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="84"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="82"/>
       <c r="Q1" s="68"/>
       <c r="R1" s="68"/>
       <c r="S1" s="68"/>
       <c r="T1" s="68"/>
       <c r="U1" s="68"/>
       <c r="V1" s="69"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="68"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="113"/>
+      <c r="Y1" s="114"/>
       <c r="Z1" s="67"/>
       <c r="AA1" s="69"/>
-      <c r="AB1" s="90">
+      <c r="AB1" s="87">
         <f>SUM(AB$23:AB$42)</f>
         <v>0</v>
       </c>
@@ -1942,7 +2139,7 @@
         <f>SUM(A$23:A$42)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="72">
+      <c r="B2" s="71">
         <f>SUM(B$30:B$35)</f>
         <v>0</v>
       </c>
@@ -1951,33 +2148,33 @@
         <f>SUM(D$23:D$42)</f>
         <v>0</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="117"/>
       <c r="H2" s="69"/>
       <c r="I2" s="68"/>
       <c r="J2" s="68"/>
       <c r="K2" s="68"/>
       <c r="L2" s="68"/>
       <c r="M2" s="68"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="84"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="82"/>
       <c r="Q2" s="68"/>
       <c r="R2" s="68"/>
       <c r="S2" s="68"/>
       <c r="T2" s="68"/>
       <c r="U2" s="68"/>
       <c r="V2" s="69"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="68"/>
+      <c r="W2" s="115"/>
+      <c r="X2" s="116"/>
+      <c r="Y2" s="117"/>
       <c r="Z2" s="67">
         <f>SUM(Z$23:Z$42)</f>
         <v>0</v>
       </c>
       <c r="AA2" s="69"/>
-      <c r="AB2" s="72">
+      <c r="AB2" s="71">
         <f>SUM(AB$30:AB$35)</f>
         <v>0</v>
       </c>
@@ -1987,261 +2184,269 @@
       </c>
     </row>
     <row r="3" spans="1:29" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="e">
+      <c r="A3" s="70" t="e">
         <f>'OC Profile'!$A$6/'OC Profile'!$A$5</f>
         <v>#NUM!</v>
       </c>
-      <c r="B3" s="71" t="e">
+      <c r="B3" s="70" t="e">
         <f>'OC Profile'!$C$6/'OC Profile'!$C$5</f>
         <v>#NUM!</v>
       </c>
       <c r="C3" s="69"/>
-      <c r="D3" s="71" t="e">
+      <c r="D3" s="70" t="e">
         <f>'OC Profile'!$E$6/'OC Profile'!$E$5</f>
         <v>#NUM!</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+      <c r="E3" s="130" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="131"/>
+      <c r="G3" s="132"/>
       <c r="H3" s="69"/>
       <c r="I3" s="68"/>
       <c r="J3" s="68"/>
       <c r="K3" s="68"/>
       <c r="L3" s="68"/>
       <c r="M3" s="68"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="84"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="82"/>
       <c r="Q3" s="68"/>
       <c r="R3" s="68"/>
       <c r="S3" s="68"/>
       <c r="T3" s="68"/>
       <c r="U3" s="68"/>
       <c r="V3" s="69"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="68"/>
-      <c r="Z3" s="71" t="e">
+      <c r="W3" s="136" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="137"/>
+      <c r="Y3" s="138"/>
+      <c r="Z3" s="70" t="e">
         <f>'OC Profile'!$K$6/'OC Profile'!$K$5</f>
         <v>#NUM!</v>
       </c>
       <c r="AA3" s="69"/>
-      <c r="AB3" s="71" t="e">
+      <c r="AB3" s="70" t="e">
         <f>'OC Profile'!$I$6/'OC Profile'!$I$5</f>
         <v>#NUM!</v>
       </c>
-      <c r="AC3" s="71" t="e">
+      <c r="AC3" s="70" t="e">
         <f>'OC Profile'!$G$6/'OC Profile'!$G$5</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="4" spans="1:29" s="18" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="78" t="e">
+      <c r="A4" s="77" t="e">
         <f>'OC Profile'!$A$5/'OC Profile'!$A$4</f>
         <v>#NUM!</v>
       </c>
-      <c r="B4" s="78" t="e">
+      <c r="B4" s="77" t="e">
         <f>'OC Profile'!$C$5/'OC Profile'!$C$4</f>
         <v>#NUM!</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="78" t="e">
+      <c r="C4" s="78"/>
+      <c r="D4" s="77" t="e">
         <f>'OC Profile'!$E$5/'OC Profile'!$E$4</f>
         <v>#NUM!</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="89" t="e">
+      <c r="E4" s="118"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="86" t="e">
         <f>$AC$2/$A$2</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P4" s="85"/>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="80"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="e">
+      <c r="P4" s="83"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="79"/>
+      <c r="S4" s="79"/>
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="139"/>
+      <c r="X4" s="140"/>
+      <c r="Y4" s="141"/>
+      <c r="Z4" s="77" t="e">
         <f>'OC Profile'!$K$5/'OC Profile'!$K$4</f>
         <v>#NUM!</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="78" t="e">
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="77" t="e">
         <f>'OC Profile'!$I$5/'OC Profile'!$I$4</f>
         <v>#NUM!</v>
       </c>
-      <c r="AC4" s="78" t="e">
+      <c r="AC4" s="77" t="e">
         <f>'OC Profile'!$G$5/'OC Profile'!$G$4</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="95" customFormat="1" ht="12" x14ac:dyDescent="0.3">
-      <c r="A5" s="91" t="s">
+    <row r="5" spans="1:29" s="92" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="A5" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="91" t="s">
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="105"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="92"/>
-      <c r="R5" s="92"/>
-      <c r="S5" s="92"/>
-      <c r="T5" s="92"/>
-      <c r="U5" s="92"/>
-      <c r="V5" s="92"/>
-      <c r="W5" s="92"/>
-      <c r="X5" s="92"/>
-      <c r="Y5" s="92"/>
-      <c r="Z5" s="91" t="s">
+      <c r="E5" s="121"/>
+      <c r="F5" s="122"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="109"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="89"/>
+      <c r="R5" s="89"/>
+      <c r="S5" s="89"/>
+      <c r="T5" s="89"/>
+      <c r="U5" s="89"/>
+      <c r="V5" s="89"/>
+      <c r="W5" s="142"/>
+      <c r="X5" s="143"/>
+      <c r="Y5" s="144"/>
+      <c r="Z5" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="AA5" s="92"/>
-      <c r="AB5" s="92"/>
-      <c r="AC5" s="91" t="s">
+      <c r="AA5" s="89"/>
+      <c r="AB5" s="89"/>
+      <c r="AC5" s="88" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="95" customFormat="1" ht="12" x14ac:dyDescent="0.3">
-      <c r="A6" s="96" t="e">
+    <row r="6" spans="1:29" s="92" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+      <c r="A6" s="93" t="e">
         <f>'OC Profile'!$A$4-'OC Profile'!$A$5</f>
         <v>#NUM!</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="96" t="e">
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="93" t="e">
         <f>'OC Profile'!$E$4-'OC Profile'!$E$5</f>
         <v>#NUM!</v>
       </c>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="93"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="94"/>
-      <c r="Q6" s="92"/>
-      <c r="R6" s="92"/>
-      <c r="S6" s="92"/>
-      <c r="T6" s="92"/>
-      <c r="U6" s="92"/>
-      <c r="V6" s="92"/>
-      <c r="W6" s="92"/>
-      <c r="X6" s="92"/>
-      <c r="Y6" s="92"/>
-      <c r="Z6" s="96" t="e">
+      <c r="E6" s="133" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="134"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="89"/>
+      <c r="R6" s="89"/>
+      <c r="S6" s="89"/>
+      <c r="T6" s="89"/>
+      <c r="U6" s="89"/>
+      <c r="V6" s="89"/>
+      <c r="W6" s="145" t="s">
+        <v>32</v>
+      </c>
+      <c r="X6" s="146"/>
+      <c r="Y6" s="147"/>
+      <c r="Z6" s="93" t="e">
         <f>'OC Profile'!$K$4-'OC Profile'!$K$5</f>
         <v>#NUM!</v>
       </c>
-      <c r="AA6" s="92"/>
-      <c r="AB6" s="92"/>
-      <c r="AC6" s="96" t="e">
+      <c r="AA6" s="89"/>
+      <c r="AB6" s="89"/>
+      <c r="AC6" s="93" t="e">
         <f>'OC Profile'!$G$4-'OC Profile'!$G$5</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="95" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="97" t="e">
+    <row r="7" spans="1:29" s="92" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="94" t="e">
         <f>'OC Profile'!$A$5-'OC Profile'!$A$6</f>
         <v>#NUM!</v>
       </c>
-      <c r="B7" s="98"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="97" t="e">
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="94" t="e">
         <f>'OC Profile'!$E$5-'OC Profile'!$E$6</f>
         <v>#NUM!</v>
       </c>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="98"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="107"/>
-      <c r="P7" s="100"/>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="98"/>
-      <c r="S7" s="98"/>
-      <c r="T7" s="98"/>
-      <c r="U7" s="98"/>
-      <c r="V7" s="98"/>
-      <c r="W7" s="98"/>
-      <c r="X7" s="98"/>
-      <c r="Y7" s="98"/>
-      <c r="Z7" s="97" t="e">
+      <c r="E7" s="124"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="95"/>
+      <c r="N7" s="96"/>
+      <c r="O7" s="111"/>
+      <c r="P7" s="97"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="95"/>
+      <c r="S7" s="95"/>
+      <c r="T7" s="95"/>
+      <c r="U7" s="95"/>
+      <c r="V7" s="95"/>
+      <c r="W7" s="100"/>
+      <c r="X7" s="101"/>
+      <c r="Y7" s="102"/>
+      <c r="Z7" s="94" t="e">
         <f>'OC Profile'!$K$5-'OC Profile'!$K$6</f>
         <v>#NUM!</v>
       </c>
-      <c r="AA7" s="98"/>
-      <c r="AB7" s="98"/>
-      <c r="AC7" s="97" t="e">
+      <c r="AA7" s="95"/>
+      <c r="AB7" s="95"/>
+      <c r="AC7" s="94" t="e">
         <f>'OC Profile'!$G$5-'OC Profile'!$G$6</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="95" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="96"/>
-      <c r="B8" s="92"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="92"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92"/>
-      <c r="N8" s="93"/>
-      <c r="O8" s="101"/>
-      <c r="P8" s="94"/>
-      <c r="Q8" s="92"/>
-      <c r="R8" s="92"/>
-      <c r="S8" s="92"/>
-      <c r="T8" s="92"/>
-      <c r="U8" s="92"/>
-      <c r="V8" s="92"/>
-      <c r="W8" s="92"/>
-      <c r="X8" s="92"/>
-      <c r="Y8" s="92"/>
-      <c r="Z8" s="96"/>
-      <c r="AA8" s="92"/>
-      <c r="AB8" s="92"/>
-      <c r="AC8" s="96"/>
+    <row r="8" spans="1:29" s="92" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="93"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="127"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="129"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="89"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="91"/>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="89"/>
+      <c r="S8" s="89"/>
+      <c r="T8" s="89"/>
+      <c r="U8" s="89"/>
+      <c r="V8" s="89"/>
+      <c r="W8" s="103"/>
+      <c r="X8" s="104"/>
+      <c r="Y8" s="105"/>
+      <c r="Z8" s="93"/>
+      <c r="AA8" s="89"/>
+      <c r="AB8" s="89"/>
+      <c r="AC8" s="93"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="24"/>
@@ -2275,41 +2480,41 @@
       <c r="AC9" s="24"/>
     </row>
     <row r="10" spans="1:29" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="102"/>
-      <c r="C10" s="102"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
-      <c r="K10" s="102"/>
-      <c r="L10" s="102"/>
-      <c r="M10" s="102"/>
-      <c r="N10" s="102"/>
-      <c r="O10" s="103" t="s">
+      <c r="A10" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="106"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="106"/>
+      <c r="G10" s="106"/>
+      <c r="H10" s="106"/>
+      <c r="I10" s="106"/>
+      <c r="J10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="106"/>
+      <c r="M10" s="106"/>
+      <c r="N10" s="106"/>
+      <c r="O10" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="P10" s="102" t="s">
+      <c r="P10" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="Q10" s="102"/>
-      <c r="R10" s="102"/>
-      <c r="S10" s="102"/>
-      <c r="T10" s="102"/>
-      <c r="U10" s="102"/>
-      <c r="V10" s="102"/>
-      <c r="W10" s="102"/>
-      <c r="X10" s="102"/>
-      <c r="Y10" s="102"/>
-      <c r="Z10" s="102"/>
-      <c r="AA10" s="102"/>
-      <c r="AB10" s="102"/>
-      <c r="AC10" s="102"/>
+      <c r="Q10" s="106"/>
+      <c r="R10" s="106"/>
+      <c r="S10" s="106"/>
+      <c r="T10" s="106"/>
+      <c r="U10" s="106"/>
+      <c r="V10" s="106"/>
+      <c r="W10" s="106"/>
+      <c r="X10" s="106"/>
+      <c r="Y10" s="106"/>
+      <c r="Z10" s="106"/>
+      <c r="AA10" s="106"/>
+      <c r="AB10" s="106"/>
+      <c r="AC10" s="106"/>
     </row>
     <row r="11" spans="1:29" s="18" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
@@ -2354,7 +2559,7 @@
       <c r="N11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="104"/>
+      <c r="O11" s="108"/>
       <c r="P11" s="22" t="s">
         <v>11</v>
       </c>
@@ -2401,7 +2606,7 @@
     <row r="12" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
-      <c r="C12" s="10"/>
+      <c r="C12" s="160"/>
       <c r="D12" s="12"/>
       <c r="E12" s="9"/>
       <c r="F12" s="16"/>
@@ -2425,14 +2630,14 @@
       <c r="X12" s="17"/>
       <c r="Y12" s="6"/>
       <c r="Z12" s="13"/>
-      <c r="AA12" s="7"/>
+      <c r="AA12" s="161"/>
       <c r="AB12" s="13"/>
       <c r="AC12" s="13"/>
     </row>
     <row r="13" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
-      <c r="C13" s="10"/>
+      <c r="C13" s="160"/>
       <c r="D13" s="12"/>
       <c r="E13" s="9"/>
       <c r="F13" s="16"/>
@@ -2456,14 +2661,14 @@
       <c r="X13" s="17"/>
       <c r="Y13" s="6"/>
       <c r="Z13" s="13"/>
-      <c r="AA13" s="7"/>
+      <c r="AA13" s="161"/>
       <c r="AB13" s="13"/>
       <c r="AC13" s="13"/>
     </row>
     <row r="14" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="10"/>
+      <c r="C14" s="160"/>
       <c r="D14" s="12"/>
       <c r="E14" s="9"/>
       <c r="F14" s="16"/>
@@ -2487,14 +2692,14 @@
       <c r="X14" s="17"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="13"/>
-      <c r="AA14" s="7"/>
+      <c r="AA14" s="161"/>
       <c r="AB14" s="13"/>
       <c r="AC14" s="13"/>
     </row>
     <row r="15" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="10"/>
+      <c r="C15" s="160"/>
       <c r="D15" s="12"/>
       <c r="E15" s="9"/>
       <c r="F15" s="16"/>
@@ -2518,14 +2723,14 @@
       <c r="X15" s="17"/>
       <c r="Y15" s="6"/>
       <c r="Z15" s="13"/>
-      <c r="AA15" s="7"/>
+      <c r="AA15" s="161"/>
       <c r="AB15" s="13"/>
       <c r="AC15" s="13"/>
     </row>
     <row r="16" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="10"/>
+      <c r="C16" s="160"/>
       <c r="D16" s="12"/>
       <c r="E16" s="9"/>
       <c r="F16" s="16"/>
@@ -2549,14 +2754,14 @@
       <c r="X16" s="17"/>
       <c r="Y16" s="6"/>
       <c r="Z16" s="13"/>
-      <c r="AA16" s="7"/>
+      <c r="AA16" s="161"/>
       <c r="AB16" s="13"/>
       <c r="AC16" s="13"/>
     </row>
     <row r="17" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
-      <c r="C17" s="10"/>
+      <c r="C17" s="160"/>
       <c r="D17" s="12"/>
       <c r="E17" s="9"/>
       <c r="F17" s="16"/>
@@ -2580,14 +2785,14 @@
       <c r="X17" s="17"/>
       <c r="Y17" s="6"/>
       <c r="Z17" s="13"/>
-      <c r="AA17" s="7"/>
+      <c r="AA17" s="161"/>
       <c r="AB17" s="13"/>
       <c r="AC17" s="13"/>
     </row>
     <row r="18" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="10"/>
+      <c r="C18" s="160"/>
       <c r="D18" s="12"/>
       <c r="E18" s="9"/>
       <c r="F18" s="16"/>
@@ -2611,14 +2816,14 @@
       <c r="X18" s="17"/>
       <c r="Y18" s="6"/>
       <c r="Z18" s="13"/>
-      <c r="AA18" s="7"/>
+      <c r="AA18" s="161"/>
       <c r="AB18" s="13"/>
       <c r="AC18" s="13"/>
     </row>
     <row r="19" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="10"/>
+      <c r="C19" s="160"/>
       <c r="D19" s="12"/>
       <c r="E19" s="9"/>
       <c r="F19" s="16"/>
@@ -2642,14 +2847,14 @@
       <c r="X19" s="17"/>
       <c r="Y19" s="6"/>
       <c r="Z19" s="13"/>
-      <c r="AA19" s="7"/>
+      <c r="AA19" s="161"/>
       <c r="AB19" s="13"/>
       <c r="AC19" s="13"/>
     </row>
     <row r="20" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="10"/>
+      <c r="C20" s="160"/>
       <c r="D20" s="12"/>
       <c r="E20" s="9"/>
       <c r="F20" s="16"/>
@@ -2673,14 +2878,14 @@
       <c r="X20" s="17"/>
       <c r="Y20" s="6"/>
       <c r="Z20" s="13"/>
-      <c r="AA20" s="7"/>
+      <c r="AA20" s="161"/>
       <c r="AB20" s="13"/>
       <c r="AC20" s="13"/>
     </row>
     <row r="21" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
-      <c r="C21" s="10"/>
+      <c r="C21" s="160"/>
       <c r="D21" s="12"/>
       <c r="E21" s="9"/>
       <c r="F21" s="16"/>
@@ -2704,14 +2909,14 @@
       <c r="X21" s="17"/>
       <c r="Y21" s="6"/>
       <c r="Z21" s="13"/>
-      <c r="AA21" s="7"/>
+      <c r="AA21" s="161"/>
       <c r="AB21" s="13"/>
       <c r="AC21" s="13"/>
     </row>
     <row r="22" spans="1:29" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="160"/>
       <c r="D22" s="12"/>
       <c r="E22" s="9"/>
       <c r="F22" s="16"/>
@@ -2735,14 +2940,14 @@
       <c r="X22" s="17"/>
       <c r="Y22" s="6"/>
       <c r="Z22" s="13"/>
-      <c r="AA22" s="7"/>
+      <c r="AA22" s="161"/>
       <c r="AB22" s="13"/>
       <c r="AC22" s="13"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
-      <c r="C23" s="10"/>
+      <c r="C23" s="160"/>
       <c r="D23" s="12"/>
       <c r="E23" s="9"/>
       <c r="F23" s="16"/>
@@ -2766,14 +2971,14 @@
       <c r="X23" s="17"/>
       <c r="Y23" s="6"/>
       <c r="Z23" s="13"/>
-      <c r="AA23" s="7"/>
+      <c r="AA23" s="161"/>
       <c r="AB23" s="13"/>
       <c r="AC23" s="13"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="10"/>
+      <c r="C24" s="160"/>
       <c r="D24" s="12"/>
       <c r="E24" s="9"/>
       <c r="F24" s="16"/>
@@ -2797,14 +3002,14 @@
       <c r="X24" s="17"/>
       <c r="Y24" s="6"/>
       <c r="Z24" s="13"/>
-      <c r="AA24" s="7"/>
+      <c r="AA24" s="161"/>
       <c r="AB24" s="13"/>
       <c r="AC24" s="13"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="10"/>
+      <c r="C25" s="160"/>
       <c r="D25" s="12"/>
       <c r="E25" s="9"/>
       <c r="F25" s="16"/>
@@ -2828,14 +3033,14 @@
       <c r="X25" s="17"/>
       <c r="Y25" s="6"/>
       <c r="Z25" s="13"/>
-      <c r="AA25" s="7"/>
+      <c r="AA25" s="161"/>
       <c r="AB25" s="13"/>
       <c r="AC25" s="13"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="10"/>
+      <c r="C26" s="160"/>
       <c r="D26" s="12"/>
       <c r="E26" s="9"/>
       <c r="F26" s="16"/>
@@ -2859,14 +3064,14 @@
       <c r="X26" s="17"/>
       <c r="Y26" s="6"/>
       <c r="Z26" s="13"/>
-      <c r="AA26" s="7"/>
+      <c r="AA26" s="161"/>
       <c r="AB26" s="13"/>
       <c r="AC26" s="13"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
-      <c r="C27" s="10"/>
+      <c r="C27" s="160"/>
       <c r="D27" s="12"/>
       <c r="E27" s="9"/>
       <c r="F27" s="16"/>
@@ -2890,14 +3095,14 @@
       <c r="X27" s="17"/>
       <c r="Y27" s="6"/>
       <c r="Z27" s="13"/>
-      <c r="AA27" s="7"/>
+      <c r="AA27" s="161"/>
       <c r="AB27" s="13"/>
       <c r="AC27" s="13"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="10"/>
+      <c r="C28" s="160"/>
       <c r="D28" s="12"/>
       <c r="E28" s="9"/>
       <c r="F28" s="16"/>
@@ -2921,14 +3126,14 @@
       <c r="X28" s="17"/>
       <c r="Y28" s="6"/>
       <c r="Z28" s="13"/>
-      <c r="AA28" s="7"/>
+      <c r="AA28" s="161"/>
       <c r="AB28" s="13"/>
       <c r="AC28" s="13"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
-      <c r="C29" s="10"/>
+      <c r="C29" s="160"/>
       <c r="D29" s="12"/>
       <c r="E29" s="9"/>
       <c r="F29" s="16"/>
@@ -2952,14 +3157,14 @@
       <c r="X29" s="17"/>
       <c r="Y29" s="6"/>
       <c r="Z29" s="13"/>
-      <c r="AA29" s="7"/>
+      <c r="AA29" s="161"/>
       <c r="AB29" s="13"/>
       <c r="AC29" s="13"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="10"/>
+      <c r="C30" s="160"/>
       <c r="D30" s="12"/>
       <c r="E30" s="9"/>
       <c r="F30" s="16"/>
@@ -2983,14 +3188,14 @@
       <c r="X30" s="17"/>
       <c r="Y30" s="6"/>
       <c r="Z30" s="13"/>
-      <c r="AA30" s="7"/>
+      <c r="AA30" s="161"/>
       <c r="AB30" s="13"/>
       <c r="AC30" s="13"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="10"/>
+      <c r="C31" s="160"/>
       <c r="D31" s="12"/>
       <c r="E31" s="9"/>
       <c r="F31" s="16"/>
@@ -3014,14 +3219,14 @@
       <c r="X31" s="17"/>
       <c r="Y31" s="6"/>
       <c r="Z31" s="13"/>
-      <c r="AA31" s="7"/>
+      <c r="AA31" s="161"/>
       <c r="AB31" s="13"/>
       <c r="AC31" s="13"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
-      <c r="C32" s="10"/>
+      <c r="C32" s="160"/>
       <c r="D32" s="12"/>
       <c r="E32" s="9"/>
       <c r="F32" s="16"/>
@@ -3045,14 +3250,14 @@
       <c r="X32" s="17"/>
       <c r="Y32" s="6"/>
       <c r="Z32" s="13"/>
-      <c r="AA32" s="7"/>
+      <c r="AA32" s="161"/>
       <c r="AB32" s="13"/>
       <c r="AC32" s="13"/>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
-      <c r="C33" s="7"/>
+      <c r="C33" s="161"/>
       <c r="D33" s="13"/>
       <c r="E33" s="6"/>
       <c r="F33" s="17"/>
@@ -3076,14 +3281,14 @@
       <c r="X33" s="16"/>
       <c r="Y33" s="9"/>
       <c r="Z33" s="12"/>
-      <c r="AA33" s="10"/>
+      <c r="AA33" s="160"/>
       <c r="AB33" s="12"/>
       <c r="AC33" s="12"/>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
-      <c r="C34" s="7"/>
+      <c r="C34" s="161"/>
       <c r="D34" s="13"/>
       <c r="E34" s="6"/>
       <c r="F34" s="17"/>
@@ -3107,14 +3312,14 @@
       <c r="X34" s="16"/>
       <c r="Y34" s="9"/>
       <c r="Z34" s="12"/>
-      <c r="AA34" s="10"/>
+      <c r="AA34" s="160"/>
       <c r="AB34" s="12"/>
       <c r="AC34" s="12"/>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
-      <c r="C35" s="7"/>
+      <c r="C35" s="161"/>
       <c r="D35" s="13"/>
       <c r="E35" s="6"/>
       <c r="F35" s="17"/>
@@ -3138,14 +3343,14 @@
       <c r="X35" s="16"/>
       <c r="Y35" s="9"/>
       <c r="Z35" s="12"/>
-      <c r="AA35" s="10"/>
+      <c r="AA35" s="160"/>
       <c r="AB35" s="12"/>
       <c r="AC35" s="12"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
-      <c r="C36" s="7"/>
+      <c r="C36" s="161"/>
       <c r="D36" s="13"/>
       <c r="E36" s="6"/>
       <c r="F36" s="17"/>
@@ -3169,14 +3374,14 @@
       <c r="X36" s="16"/>
       <c r="Y36" s="9"/>
       <c r="Z36" s="12"/>
-      <c r="AA36" s="10"/>
+      <c r="AA36" s="160"/>
       <c r="AB36" s="12"/>
       <c r="AC36" s="12"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
-      <c r="C37" s="7"/>
+      <c r="C37" s="161"/>
       <c r="D37" s="13"/>
       <c r="E37" s="6"/>
       <c r="F37" s="17"/>
@@ -3200,14 +3405,14 @@
       <c r="X37" s="16"/>
       <c r="Y37" s="9"/>
       <c r="Z37" s="12"/>
-      <c r="AA37" s="10"/>
+      <c r="AA37" s="160"/>
       <c r="AB37" s="12"/>
       <c r="AC37" s="12"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
-      <c r="C38" s="7"/>
+      <c r="C38" s="161"/>
       <c r="D38" s="13"/>
       <c r="E38" s="6"/>
       <c r="F38" s="17"/>
@@ -3231,14 +3436,14 @@
       <c r="X38" s="16"/>
       <c r="Y38" s="9"/>
       <c r="Z38" s="12"/>
-      <c r="AA38" s="10"/>
+      <c r="AA38" s="160"/>
       <c r="AB38" s="12"/>
       <c r="AC38" s="12"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
-      <c r="C39" s="7"/>
+      <c r="C39" s="161"/>
       <c r="D39" s="13"/>
       <c r="E39" s="6"/>
       <c r="F39" s="17"/>
@@ -3262,14 +3467,14 @@
       <c r="X39" s="16"/>
       <c r="Y39" s="9"/>
       <c r="Z39" s="12"/>
-      <c r="AA39" s="10"/>
+      <c r="AA39" s="160"/>
       <c r="AB39" s="12"/>
       <c r="AC39" s="12"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
-      <c r="C40" s="7"/>
+      <c r="C40" s="161"/>
       <c r="D40" s="13"/>
       <c r="E40" s="6"/>
       <c r="F40" s="17"/>
@@ -3293,14 +3498,14 @@
       <c r="X40" s="16"/>
       <c r="Y40" s="9"/>
       <c r="Z40" s="12"/>
-      <c r="AA40" s="10"/>
+      <c r="AA40" s="160"/>
       <c r="AB40" s="12"/>
       <c r="AC40" s="12"/>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
-      <c r="C41" s="7"/>
+      <c r="C41" s="161"/>
       <c r="D41" s="13"/>
       <c r="E41" s="6"/>
       <c r="F41" s="17"/>
@@ -3324,14 +3529,14 @@
       <c r="X41" s="16"/>
       <c r="Y41" s="9"/>
       <c r="Z41" s="12"/>
-      <c r="AA41" s="10"/>
+      <c r="AA41" s="160"/>
       <c r="AB41" s="12"/>
       <c r="AC41" s="12"/>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
-      <c r="C42" s="7"/>
+      <c r="C42" s="161"/>
       <c r="D42" s="13"/>
       <c r="E42" s="6"/>
       <c r="F42" s="17"/>
@@ -3355,14 +3560,14 @@
       <c r="X42" s="16"/>
       <c r="Y42" s="9"/>
       <c r="Z42" s="12"/>
-      <c r="AA42" s="10"/>
+      <c r="AA42" s="160"/>
       <c r="AB42" s="12"/>
       <c r="AC42" s="12"/>
     </row>
     <row r="43" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
-      <c r="C43" s="7"/>
+      <c r="C43" s="161"/>
       <c r="D43" s="13"/>
       <c r="E43" s="6"/>
       <c r="F43" s="17"/>
@@ -3386,14 +3591,14 @@
       <c r="X43" s="16"/>
       <c r="Y43" s="9"/>
       <c r="Z43" s="12"/>
-      <c r="AA43" s="10"/>
+      <c r="AA43" s="160"/>
       <c r="AB43" s="12"/>
       <c r="AC43" s="12"/>
     </row>
     <row r="44" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
-      <c r="C44" s="7"/>
+      <c r="C44" s="161"/>
       <c r="D44" s="13"/>
       <c r="E44" s="6"/>
       <c r="F44" s="17"/>
@@ -3417,14 +3622,14 @@
       <c r="X44" s="16"/>
       <c r="Y44" s="9"/>
       <c r="Z44" s="12"/>
-      <c r="AA44" s="10"/>
+      <c r="AA44" s="160"/>
       <c r="AB44" s="12"/>
       <c r="AC44" s="12"/>
     </row>
     <row r="45" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
-      <c r="C45" s="7"/>
+      <c r="C45" s="161"/>
       <c r="D45" s="13"/>
       <c r="E45" s="6"/>
       <c r="F45" s="17"/>
@@ -3448,14 +3653,14 @@
       <c r="X45" s="16"/>
       <c r="Y45" s="9"/>
       <c r="Z45" s="12"/>
-      <c r="AA45" s="10"/>
+      <c r="AA45" s="160"/>
       <c r="AB45" s="12"/>
       <c r="AC45" s="12"/>
     </row>
     <row r="46" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
-      <c r="C46" s="7"/>
+      <c r="C46" s="161"/>
       <c r="D46" s="13"/>
       <c r="E46" s="6"/>
       <c r="F46" s="17"/>
@@ -3479,14 +3684,14 @@
       <c r="X46" s="16"/>
       <c r="Y46" s="9"/>
       <c r="Z46" s="12"/>
-      <c r="AA46" s="10"/>
+      <c r="AA46" s="160"/>
       <c r="AB46" s="12"/>
       <c r="AC46" s="12"/>
     </row>
     <row r="47" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
-      <c r="C47" s="7"/>
+      <c r="C47" s="161"/>
       <c r="D47" s="13"/>
       <c r="E47" s="6"/>
       <c r="F47" s="17"/>
@@ -3510,14 +3715,14 @@
       <c r="X47" s="16"/>
       <c r="Y47" s="9"/>
       <c r="Z47" s="12"/>
-      <c r="AA47" s="10"/>
+      <c r="AA47" s="160"/>
       <c r="AB47" s="12"/>
       <c r="AC47" s="12"/>
     </row>
     <row r="48" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
-      <c r="C48" s="7"/>
+      <c r="C48" s="161"/>
       <c r="D48" s="13"/>
       <c r="E48" s="6"/>
       <c r="F48" s="17"/>
@@ -3541,14 +3746,14 @@
       <c r="X48" s="16"/>
       <c r="Y48" s="9"/>
       <c r="Z48" s="12"/>
-      <c r="AA48" s="10"/>
+      <c r="AA48" s="160"/>
       <c r="AB48" s="12"/>
       <c r="AC48" s="12"/>
     </row>
     <row r="49" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
-      <c r="C49" s="7"/>
+      <c r="C49" s="161"/>
       <c r="D49" s="13"/>
       <c r="E49" s="6"/>
       <c r="F49" s="17"/>
@@ -3572,14 +3777,14 @@
       <c r="X49" s="16"/>
       <c r="Y49" s="9"/>
       <c r="Z49" s="12"/>
-      <c r="AA49" s="10"/>
+      <c r="AA49" s="160"/>
       <c r="AB49" s="12"/>
       <c r="AC49" s="12"/>
     </row>
     <row r="50" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
-      <c r="C50" s="7"/>
+      <c r="C50" s="161"/>
       <c r="D50" s="13"/>
       <c r="E50" s="6"/>
       <c r="F50" s="17"/>
@@ -3603,14 +3808,14 @@
       <c r="X50" s="16"/>
       <c r="Y50" s="9"/>
       <c r="Z50" s="12"/>
-      <c r="AA50" s="10"/>
+      <c r="AA50" s="160"/>
       <c r="AB50" s="12"/>
       <c r="AC50" s="12"/>
     </row>
     <row r="51" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
-      <c r="C51" s="7"/>
+      <c r="C51" s="161"/>
       <c r="D51" s="13"/>
       <c r="E51" s="6"/>
       <c r="F51" s="17"/>
@@ -3634,14 +3839,14 @@
       <c r="X51" s="16"/>
       <c r="Y51" s="9"/>
       <c r="Z51" s="12"/>
-      <c r="AA51" s="10"/>
+      <c r="AA51" s="160"/>
       <c r="AB51" s="12"/>
       <c r="AC51" s="12"/>
     </row>
     <row r="52" spans="1:29" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
-      <c r="C52" s="7"/>
+      <c r="C52" s="161"/>
       <c r="D52" s="13"/>
       <c r="E52" s="6"/>
       <c r="F52" s="17"/>
@@ -3665,22 +3870,32 @@
       <c r="X52" s="16"/>
       <c r="Y52" s="9"/>
       <c r="Z52" s="12"/>
-      <c r="AA52" s="10"/>
+      <c r="AA52" s="160"/>
       <c r="AB52" s="12"/>
       <c r="AC52" s="12"/>
     </row>
     <row r="53" spans="1:29" collapsed="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="14">
+    <mergeCell ref="W1:Y2"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="W4:Y5"/>
+    <mergeCell ref="W6:Y6"/>
+    <mergeCell ref="E1:G2"/>
+    <mergeCell ref="E4:G5"/>
+    <mergeCell ref="E7:G8"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="W7:Y8"/>
     <mergeCell ref="A10:N10"/>
     <mergeCell ref="O10:O11"/>
     <mergeCell ref="P10:AC10"/>
     <mergeCell ref="O5:O7"/>
   </mergeCells>
   <conditionalFormatting sqref="A33:A52">
-    <cfRule type="top10" dxfId="31" priority="34" rank="1"/>
-    <cfRule type="top10" dxfId="30" priority="35" rank="2"/>
-    <cfRule type="top10" dxfId="29" priority="36" rank="3"/>
+    <cfRule type="top10" dxfId="31" priority="36" rank="3"/>
+    <cfRule type="top10" dxfId="30" priority="34" rank="1"/>
+    <cfRule type="top10" dxfId="29" priority="35" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B4 D3:D4 Z3:Z4 AB3:AC4">
     <cfRule type="cellIs" dxfId="28" priority="4" operator="greaterThan">
@@ -3700,6 +3915,18 @@
     <cfRule type="top10" dxfId="24" priority="22" rank="1"/>
     <cfRule type="top10" dxfId="23" priority="23" rank="2"/>
     <cfRule type="top10" dxfId="22" priority="24" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C42">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="-2.5"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="2.5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:D52">
     <cfRule type="top10" dxfId="21" priority="28" rank="1"/>
@@ -3728,28 +3955,6 @@
     <cfRule type="top10" dxfId="7" priority="26" rank="2"/>
     <cfRule type="top10" dxfId="6" priority="27" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB12:AB32">
-    <cfRule type="top10" dxfId="5" priority="19" rank="1"/>
-    <cfRule type="top10" dxfId="4" priority="20" rank="2"/>
-    <cfRule type="top10" dxfId="3" priority="21" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC12:AC32">
-    <cfRule type="top10" dxfId="2" priority="31" rank="1"/>
-    <cfRule type="top10" dxfId="1" priority="32" rank="2"/>
-    <cfRule type="top10" dxfId="0" priority="33" rank="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22:C42">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="-2.5"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="2.5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AA22:AA42">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -3761,6 +3966,16 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB12:AB32">
+    <cfRule type="top10" dxfId="5" priority="21" rank="3"/>
+    <cfRule type="top10" dxfId="4" priority="19" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="20" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC12:AC32">
+    <cfRule type="top10" dxfId="2" priority="31" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="32" rank="2"/>
+    <cfRule type="top10" dxfId="0" priority="33" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -3886,6 +4101,102 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{B0A96CAD-C9F8-4597-864F-D5792C40DFA8}">
+          <x14:colorSeries theme="3"/>
+          <x14:colorNegative theme="9"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="8"/>
+          <x14:colorFirst theme="4"/>
+          <x14:colorLast theme="5"/>
+          <x14:colorHigh theme="6"/>
+          <x14:colorLow theme="7"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Option Chain'!$E$22:$E$42</xm:f>
+              <xm:sqref>E1</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{C36C5E2A-BD6A-4780-9911-55F8298D6C0B}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Option Chain'!$Y$22:$Y$42</xm:f>
+              <xm:sqref>W1</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{EE37D2D2-71BF-4081-970C-48958B68C958}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Option Chain'!$E$22:$E$32</xm:f>
+              <xm:sqref>E4</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{FEBE446C-4AAC-4EF8-A775-2D5CED98CE2A}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Option Chain'!$Y$33:$Y$42</xm:f>
+              <xm:sqref>W7</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{45739CE5-1DED-4E4A-875D-2A225C469B05}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Option Chain'!$E$33:$E$42</xm:f>
+              <xm:sqref>E7</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{323A9212-D2C9-4135-BE67-5C68EE8FAA82}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Option Chain'!$Y$22:$Y$32</xm:f>
+              <xm:sqref>W4</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
@@ -3918,50 +4229,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="149" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="109"/>
-      <c r="Q1" s="110" t="s">
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
+      <c r="L1" s="149"/>
+      <c r="M1" s="149"/>
+      <c r="N1" s="149"/>
+      <c r="O1" s="149"/>
+      <c r="Q1" s="150" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="111"/>
+      <c r="R1" s="151"/>
     </row>
     <row r="2" spans="1:18" s="29" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="108" t="s">
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="113"/>
+      <c r="Q2" s="152"/>
+      <c r="R2" s="153"/>
     </row>
     <row r="3" spans="1:18" s="29" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
@@ -4006,9 +4317,9 @@
       <c r="N3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="108"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73" t="s">
+      <c r="O3" s="148"/>
+      <c r="Q3" s="72"/>
+      <c r="R3" s="72" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4073,10 +4384,10 @@
         <f>'Option Chain'!O12</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="74" t="s">
+      <c r="Q4" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="76">
+      <c r="R4" s="75">
         <f>'Option Chain'!$B$1</f>
         <v>0</v>
       </c>
@@ -4142,10 +4453,10 @@
         <f>'Option Chain'!O13</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="75" t="s">
+      <c r="Q5" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="R5" s="77">
+      <c r="R5" s="76">
         <f>'Option Chain'!$AB$1</f>
         <v>0</v>
       </c>
@@ -4211,10 +4522,10 @@
         <f>'Option Chain'!O14</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="74" t="s">
+      <c r="Q6" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="76">
+      <c r="R6" s="75">
         <f>'Option Chain'!$B$2</f>
         <v>0</v>
       </c>
@@ -4280,10 +4591,10 @@
         <f>'Option Chain'!O15</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="75" t="s">
+      <c r="Q7" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="R7" s="77">
+      <c r="R7" s="76">
         <f>'Option Chain'!$AB$2</f>
         <v>0</v>
       </c>
@@ -5369,44 +5680,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="28" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="154" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="116"/>
-      <c r="N1" s="110" t="s">
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="155"/>
+      <c r="I1" s="155"/>
+      <c r="J1" s="155"/>
+      <c r="K1" s="155"/>
+      <c r="L1" s="156"/>
+      <c r="N1" s="150" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="111"/>
+      <c r="O1" s="151"/>
     </row>
     <row r="2" spans="1:15" s="18" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="117" t="s">
+      <c r="B2" s="158"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="157" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="119"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="113"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="159"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="153"/>
     </row>
     <row r="3" spans="1:15" s="18" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="35" t="s">

</xml_diff>